<commit_message>
rescructure and code edits
</commit_message>
<xml_diff>
--- a/NetRealmsNanSetup/nanDECK/cards.xlsx
+++ b/NetRealmsNanSetup/nanDECK/cards.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Lands" sheetId="1" r:id="rId1"/>
+    <sheet name="WorldWeavers" sheetId="2" r:id="rId2"/>
+    <sheet name="Units" sheetId="3" r:id="rId3"/>
+    <sheet name="Relics" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -616,12 +617,217 @@
   <si>
     <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Gaming\CrimsonCircuitWyvern.jpeg</t>
   </si>
+  <si>
+    <t>Xieon, Lord of the Code</t>
+  </si>
+  <si>
+    <t>Ashke, Seductress of the Server</t>
+  </si>
+  <si>
+    <t>ProtoMyke, Sculptor of Realms</t>
+  </si>
+  <si>
+    <t>Vexis, Whisperer of Shadows</t>
+  </si>
+  <si>
+    <t>Lyra, Harbinger of Discord</t>
+  </si>
+  <si>
+    <t>Legendary WorldWeaver - Xieon</t>
+  </si>
+  <si>
+    <t>Legendary WorldWeaver - Ashke</t>
+  </si>
+  <si>
+    <t>Legendary WorldWeaver - ProtoMyke</t>
+  </si>
+  <si>
+    <t>Legendary WorldWeaver - Vexis</t>
+  </si>
+  <si>
+    <t>Legendary WorldWeaver - Lyra</t>
+  </si>
+  <si>
+    <t>Fragmented Disk</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\frames\frame_common.png</t>
+  </si>
+  <si>
+    <t>Corrupted Mirror</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\frames\frame_uncommon.png</t>
+  </si>
+  <si>
+    <t>Holo-Key</t>
+  </si>
+  <si>
+    <t>Defective Processon</t>
+  </si>
+  <si>
+    <t>Glitched Beacon</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\frames\frame_rare.png</t>
+  </si>
+  <si>
+    <t>Static Core</t>
+  </si>
+  <si>
+    <t>Broken Modulator</t>
+  </si>
+  <si>
+    <t>Crash Helm</t>
+  </si>
+  <si>
+    <t>Data Worm</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\frames\frame_epic.png</t>
+  </si>
+  <si>
+    <t>Error Generator</t>
+  </si>
+  <si>
+    <t>Loop Disk</t>
+  </si>
+  <si>
+    <t>Misaligned Node</t>
+  </si>
+  <si>
+    <t>Corrupting Lense</t>
+  </si>
+  <si>
+    <t>Patchwork Circuit</t>
+  </si>
+  <si>
+    <t>Digital Relic</t>
+  </si>
+  <si>
+    <t>Relic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap: Add one mana of any color. When you use this mana to upload a Program, lose 1 Integrity.
+</t>
+  </si>
+  <si>
+    <t>Tap: Add one energy of any Node, When you use this energy to upload a Program, lose 1 Integrity</t>
+  </si>
+  <si>
+    <t>Tap: Copy target Unit's abilities untill end of turn, You lose 1 Integrity</t>
+  </si>
+  <si>
+    <t>Tape" Search your archive for a Program and put it into your hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Its data may be incomplete, but its potential remains infinite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It reflects more than just an image—it reveals possibilities you wish it wouldn’t. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The doors it unlocks are endless. Just don’t expect to know what’s on the other side. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faulty, yet functional. The Grid's greatest inventions are often its accidents. </t>
+  </si>
+  <si>
+    <t>Its light guides the lost, but its glow is tainted with chaos."</t>
+  </si>
+  <si>
+    <t>Its light guides the lost, but its glow is tainted with chaos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An unstable core that turns invulnerability into vulnerability. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Even when malfunctioning, its power redefines the battlefield. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The last line of defense for those braving the Grid’s chaos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It burrows through archives, leaving a trail of corrupted knowledge. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">From the heart of chaos, it rewrites the rules of existence." </t>
+  </si>
+  <si>
+    <t>From the heart of chaos, it rewrites the rules of existence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It plays the same song over and over, each time in a different key. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It channels energy unpredictably, but somehow it always works out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What it shows is not always true, but it’s always dangerous. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A cobbled-together relic, its true strength lies in its imperfections. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A piece of history, its data laced with secrets no one dares to decode. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap: Draw a card, then discard a card. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units you control with Glitch energy gain +1/+0. </t>
+  </si>
+  <si>
+    <t>Tap: Target Unit loses Shielded until end of turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap: Switch the attack and defense of target Unit until end of turn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipped Unit gains +1/+2. Whenever it blocks, lose 1 Integrity. </t>
+  </si>
+  <si>
+    <t>Equipped Unit gains +1/+2. Whenever it blocks, lose 1 Integrity.  Tap 2 to Equip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whenever a Unit attacks, its controller mills 2 cards. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap: Exile the top card of each player’s archive. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap: Return target card from your exile to your hand. Lose 2 Integrity. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add GG. Spend this Energy only to upload Programs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap: Add GG. Spend this Energy only to upload Programs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tap: Target Unit gains -1/-0 until end of turn. </t>
+  </si>
+  <si>
+    <t>Whenever you upload a Program, gain 1 Energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the beginning of your upload, draw a card, then discard a card. </t>
+  </si>
+  <si>
+    <t>C:\Users\Twizt\OneDrive\Desktop\Github\NetRealm-XGCTCG\NetRealmsNanSetup\nanDECK\netrealms\cards\Glitch\Relic</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,16 +878,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Segoe UI"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="Segoe UI"/>
+      <color rgb="FF000000"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7DEE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95B3D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF548ED5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DB3E3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -689,11 +933,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" applyAlignment="1" xfId="0">
       <alignment wrapText="1"/>
@@ -721,6 +985,22 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" applyAlignment="1" xfId="0">
       <alignment/>
     </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="4" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="5" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="6" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="6" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" applyAlignment="1" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,21 +1317,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="C23">
-      <selection activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView workbookViewId="0" topLeftCell="A9">
+      <selection activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="63.44140625" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1" style="6"/>
-    <col min="7" max="7" width="27" customWidth="1" style="6"/>
-    <col min="8" max="8" width="27" customWidth="1" style="6"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
+    <col min="6" max="6" width="85.109375" customWidth="1" style="6" bestFit="1"/>
+    <col min="7" max="7" width="81.21875" customWidth="1" style="6" bestFit="1"/>
+    <col min="8" max="8" width="137.6640625" customWidth="1" style="6"/>
+    <col min="9" max="9" width="6.77734375" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" customWidth="1"/>
+    <col min="11" max="11" width="72.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1397,76 +1679,76 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>195</v>
-      </c>
-      <c r="D30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J30">
-        <v>5</v>
-      </c>
-      <c r="K30" t="s">
-        <v>47</v>
-      </c>
-    </row>
+    <row r="30" customFormat="1" s="0"/>
     <row r="31">
-      <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" t="s">
-        <v>197</v>
-      </c>
-      <c r="D31">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I31">
-        <v>5</v>
-      </c>
-      <c r="J31">
-        <v>4</v>
-      </c>
-      <c r="K31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="33">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="37" customFormat="1" s="0"/>
+    <row r="38">
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="40" customFormat="1" s="0"/>
+    <row r="41">
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42">
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43">
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44">
+      <c r="F44" s="4"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45">
+      <c r="F45" s="4"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46">
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47">
+      <c r="F47" s="4"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48">
+      <c r="F48" s="4"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49">
+      <c r="F49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50">
+      <c r="F50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51">
+      <c r="F51" s="4"/>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52">
+      <c r="F52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53">
+      <c r="F53" s="4"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54">
+      <c r="K54" s="4"/>
+    </row>
+    <row r="55">
+      <c r="F55" s="4"/>
+      <c r="K55" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1477,10 +1759,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="61.77734375" customWidth="1"/>
+    <col min="3" max="3" width="59.77734375" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" width="31.77734375" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" width="80.109375" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" width="81.21875" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" width="134.33203125" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" width="48.33203125" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1489,10 +1908,412 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" width="59.88671875" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" width="70.44140625" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" width="5.5546875" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" width="85.109375" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" width="49.5546875" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" width="84.21875" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" width="72.77734375" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetViews>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="61.109375" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" width="70.44140625" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" width="80.33203125" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" width="63.109375" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2" t="s">
+        <v>229</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F3" t="s">
+        <v>230</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" t="s">
+        <v>231</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" t="s">
+        <v>251</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" t="s">
+        <v>211</v>
+      </c>
+      <c r="E14" t="s">
+        <v>227</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" t="s">
+        <v>227</v>
+      </c>
+      <c r="F15" t="s">
+        <v>261</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Drama and Creep Unit Update
</commit_message>
<xml_diff>
--- a/NetRealmsNanSetup/nanDECK/cards.xlsx
+++ b/NetRealmsNanSetup/nanDECK/cards.xlsx
@@ -2130,6 +2130,528 @@
   </si>
   <si>
     <t>Glitch Unit</t>
+  </si>
+  <si>
+    <t>When Fragmented Marionette enters the Grid, mill 2 cards.</t>
+  </si>
+  <si>
+    <t>It dances to a broken rhythm, never finding its strings.</t>
+  </si>
+  <si>
+    <t>Flying. Whenever Data Phantom deals damage to a player, they exile the top card of their archive.</t>
+  </si>
+  <si>
+    <t>It feeds on what you’ll never see again.</t>
+  </si>
+  <si>
+    <t>Whenever Looped Rogue attacks, it phases out until your next turn.</t>
+  </si>
+  <si>
+    <t>When System Eraser enters the Grid, exile up to two target Units.</t>
+  </si>
+  <si>
+    <t>Whenever Patchwork Soldier is damaged, its controller mills 1 card.</t>
+  </si>
+  <si>
+    <t>Tap: Target Unit takes 1 Damage.</t>
+  </si>
+  <si>
+    <t>Null Stalker can’t be blocked by Units with Shielded.</t>
+  </si>
+  <si>
+    <t>Null Stalker can’t be blocked.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, exile Overclocked Harbinger.</t>
+  </si>
+  <si>
+    <t>When Virus Spawn enters the Grid, create a 1/1 “Infected Token.”</t>
+  </si>
+  <si>
+    <t>Whenever Recursive Assassin destroys a Unit, return it to your hand.</t>
+  </si>
+  <si>
+    <t>When Proxy Saboteur enters the Grid, destroy target Relic.</t>
+  </si>
+  <si>
+    <t>Haste. Shard Runner deals 1 damage to its controller at the end of each turn.</t>
+  </si>
+  <si>
+    <t>Trample. When Glitched Colossus attacks, mill 3 cards.</t>
+  </si>
+  <si>
+    <t>Whenever Errorbound Wraith is targeted by a spell, its controller loses 1 Integrity.</t>
+  </si>
+  <si>
+    <t>First strike. Whenever Glitchborn Knight deals combat damage, exile the top card of its controller’s archive.</t>
+  </si>
+  <si>
+    <t>Tap: Target Unit gains +1/+1 and becomes Glitched until end of turn.</t>
+  </si>
+  <si>
+    <t>Other Glitched Units you control gain +1/+1.</t>
+  </si>
+  <si>
+    <t>Whenever Anomaly Hunter enters the Grid, target opponent reveals their hand. You may exile a card from it until Anomaly Hunter leaves the Grid.</t>
+  </si>
+  <si>
+    <t>Whenever Codebreaker Sentinel attacks, you may return a Glitched card from your exile to your archive.</t>
+  </si>
+  <si>
+    <t>Flying, Trample. When Corrupted Avatar enters the Grid, mill 5 cards.</t>
+  </si>
+  <si>
+    <t>An ancient presence, awakened and broken.</t>
+  </si>
+  <si>
+    <t>It unravels the mysteries of lost data.</t>
+  </si>
+  <si>
+    <t>It seeks out inconsistencies and eliminates them.</t>
+  </si>
+  <si>
+    <t>It controls the chaos, bending it to its will.</t>
+  </si>
+  <si>
+    <t>It rewrites the code of reality to its advantage.</t>
+  </si>
+  <si>
+    <t>Its blade cuts through code and reality alike.</t>
+  </si>
+  <si>
+    <t>Touch it, and you’ll share its curse.</t>
+  </si>
+  <si>
+    <t>Its steps rewrite the battlefield.</t>
+  </si>
+  <si>
+    <t>Fast, unstable, and unpredictable.</t>
+  </si>
+  <si>
+    <t>It doesn’t knock—it deletes.</t>
+  </si>
+  <si>
+    <t>You can’t kill what’s already been rewritten.</t>
+  </si>
+  <si>
+    <t>One glitch leads to many.</t>
+  </si>
+  <si>
+    <t>Too much power burns away too quickly.</t>
+  </si>
+  <si>
+    <t>No shield can stop the void</t>
+  </si>
+  <si>
+    <t>Small, silent, and devastating.</t>
+  </si>
+  <si>
+    <t>Built from scraps, it still finds a way to fight.</t>
+  </si>
+  <si>
+    <t>All it leaves behind is the absence of what once was.</t>
+  </si>
+  <si>
+    <t>You’ll never catch it, but it will find you.</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\ProjectN3M3SIS.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\ProjectL1CK3R</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\FragmentedMarionette</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\DataPhantom</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\LoopedRogue</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\ProjectL1CK3R.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\FragmentedMarionette.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\DataPhantom.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\LoopedRogue.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\SystemEraser.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\PatchworkSoldier.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\DisruptorDrone.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\NullStalker.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\OverclockedHarbinger.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\VirusSpawn.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\RecursiveAssassin.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\ProxySaboteur.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\ShardRunner.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\GlitchedColossus.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\ErrorboundWraith.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\GlitchbornKnight.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\StaticWeaver.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\DistortedOverseer.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\AnomalyHunter.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\CodebreakerSentinel.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Glitch\Units\CorruptedAvatar.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Creep\Relic\InvisibleHandshake.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Creep\Relic\PhantomPing.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\Xieon.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\Ashke.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\ProtoMyke.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\Vexis.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\Lyra.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\Ashke.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\ProtoMyke.jpg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\worldweavers\Xieon.jpg</t>
+  </si>
+  <si>
+    <t>Cost6</t>
+  </si>
+  <si>
+    <t>Digital Phoenix</t>
+  </si>
+  <si>
+    <t>Overclocked Hacker</t>
+  </si>
+  <si>
+    <t>Logic Sentinel</t>
+  </si>
+  <si>
+    <t>Core Guardian</t>
+  </si>
+  <si>
+    <t>Codebreaker Thief</t>
+  </si>
+  <si>
+    <t>Hexcode Serpent</t>
+  </si>
+  <si>
+    <t>Encrypted Courier</t>
+  </si>
+  <si>
+    <t>Patchwork Analyzer</t>
+  </si>
+  <si>
+    <t>Gridwalker Adept</t>
+  </si>
+  <si>
+    <t>Codebound Sentinel</t>
+  </si>
+  <si>
+    <t>Assembler Bot</t>
+  </si>
+  <si>
+    <t>Recursive Construct</t>
+  </si>
+  <si>
+    <t>Protocol Enforcer</t>
+  </si>
+  <si>
+    <t>Firewall Golem</t>
+  </si>
+  <si>
+    <t>Logic Arbiter</t>
+  </si>
+  <si>
+    <t>Code Harvester</t>
+  </si>
+  <si>
+    <t>Quantum Hacker</t>
+  </si>
+  <si>
+    <t>Debugger Infiltrator</t>
+  </si>
+  <si>
+    <t>Byte Sentinel</t>
+  </si>
+  <si>
+    <t>Syntax Slicer</t>
+  </si>
+  <si>
+    <t>Algorithmic Dragon</t>
+  </si>
+  <si>
+    <t>Cipher Guardian</t>
+  </si>
+  <si>
+    <t>Codeweaver Adept</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\CodeweaverAdept.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\CipherGuardian.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\AlgorithmicDragon.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\SyntaxSlicer.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\ByteSentinel.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\DebuggerInfiltrator.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\QuantumHacker.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\CodeHarvester.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\LogicArbiter.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\FirewallGolem.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\ProtocolEnforcer.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\RecursiveConstruct.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\AssemblerBot.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\CodeboundSentinel.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\GridwalkerAdept.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\PatchworkAnalyzer.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\EncryptedCourier.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\HexcodeSerpent.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\CodebreakerThief.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\CoreGuardian.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\LogicSentinel.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\OverclockedHacker.jpeg</t>
+  </si>
+  <si>
+    <t>C:\Users\TK\Desktop\nanDECK\netrealms\cards\Code\Units\DigitalPhoenix.jpeg</t>
+  </si>
+  <si>
+    <t>Code Unit</t>
+  </si>
+  <si>
+    <t>From the ashes of broken code, it rises anew.</t>
+  </si>
+  <si>
+    <t>Flying. When Digital Phoenix is destroyed, return it to the Grid with a +1/+1 counter.</t>
+  </si>
+  <si>
+    <t>Haste. At the end of your turn, exile Overclocked Hacker.</t>
+  </si>
+  <si>
+    <t>Tap: Add 1C for each Code Unit you control.</t>
+  </si>
+  <si>
+    <t>Tap: Prevent the next 2 damage that would be dealt to any Unit this turn.</t>
+  </si>
+  <si>
+    <t>Tap: Exile the top card of an opponent’s archive. You may play it until the end of your turn.</t>
+  </si>
+  <si>
+    <t>Deathtouch</t>
+  </si>
+  <si>
+    <t>When Encrypted Courier enters the Grid, draw a card.</t>
+  </si>
+  <si>
+    <t>Tap: Look at the top two cards of your archive. You may exile one of them.</t>
+  </si>
+  <si>
+    <t>Whenever Gridwalker Adept deals combat damage, scry 1.</t>
+  </si>
+  <si>
+    <t>Shielded. Whenever Codebound Sentinel is dealt damage, exile the top card of your archive.</t>
+  </si>
+  <si>
+    <t>Tap: Create a 1/1 Code Fragment Unit.</t>
+  </si>
+  <si>
+    <t>Whenever Recursive Construct is destroyed, return it to the Grid at the start of your next turn.</t>
+  </si>
+  <si>
+    <t>Tap: Target Unit loses its abilities until end of turn.</t>
+  </si>
+  <si>
+    <t>When Firewall Golem enters the Grid, target opponent’s next attack is negated.</t>
+  </si>
+  <si>
+    <t>Whenever Logic Arbiter deals combat damage, you may draw a card.</t>
+  </si>
+  <si>
+    <t>Whenever Code Harvester enters the Grid, you gain 1C.</t>
+  </si>
+  <si>
+    <t>Tap: Look at the top three cards of your archive. You may rearrange them in any order.</t>
+  </si>
+  <si>
+    <t>Whenever Debugger Infiltrator attacks, exile the top card of your opponent's archive.</t>
+  </si>
+  <si>
+    <t>Tap: Add 1C to your energy pool.</t>
+  </si>
+  <si>
+    <t>First strike.</t>
+  </si>
+  <si>
+    <t>Flying. Whenever Algorithmic Dragon deals damage to a player, search your archive for a Relic card and add it to your hand.</t>
+  </si>
+  <si>
+    <t>Shielded. (This Unit can’t be targeted by your opponent’s abilities.)</t>
+  </si>
+  <si>
+    <t>Tap: Target Unit gains +1/+1 until end of turn.</t>
+  </si>
+  <si>
+    <t>It burns through the system, leaving nothing but a trail of chaos.</t>
+  </si>
+  <si>
+    <t>Its logic is the foundation of the Grid’s strength.</t>
+  </si>
+  <si>
+    <t>The core must not fall, no matter the cost.</t>
+  </si>
+  <si>
+    <t>The Grid’s secrets are mine for the taking.</t>
+  </si>
+  <si>
+    <t>A single misstep, and it will devour you whole.</t>
+  </si>
+  <si>
+    <t>The message always arrives, no matter the danger.</t>
+  </si>
+  <si>
+    <t>It scans for anomalies and potential threats with surgical precision.</t>
+  </si>
+  <si>
+    <t>The Grid is an endless maze, but they walk it with ease.</t>
+  </si>
+  <si>
+    <t>It guards the Grid, even at the cost of its own integrity.</t>
+  </si>
+  <si>
+    <t>From one comes many.</t>
+  </si>
+  <si>
+    <t>Its loops are eternal.</t>
+  </si>
+  <si>
+    <t>All anomalies will be contained.</t>
+  </si>
+  <si>
+    <t>No intruder can pass through its watchful eye.</t>
+  </si>
+  <si>
+    <t>The logic is undeniable.</t>
+  </si>
+  <si>
+    <t>The Grid rewards those who work within its bounds.</t>
+  </si>
+  <si>
+    <t>Reality is just a sequence waiting to be rewritten.</t>
+  </si>
+  <si>
+    <t>Nothing escapes its scrutiny.</t>
+  </si>
+  <si>
+    <t>Every line of code serves the greater Grid.</t>
+  </si>
+  <si>
+    <t>It carves through logic with precision.</t>
+  </si>
+  <si>
+    <t>In its wings lies the knowledge of a thousand solutions.</t>
+  </si>
+  <si>
+    <t>An unbreakable cipher stands between chaos and order.</t>
+  </si>
+  <si>
+    <t>With each thread woven, the Grid grows stronger.</t>
   </si>
 </sst>
 </file>
@@ -3334,20 +3856,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView workbookViewId="0" topLeftCell="C1">
+      <selection activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="26.109375" customWidth="1"/>
-    <col min="2" max="2" width="61.77734375" customWidth="1"/>
-    <col min="3" max="3" width="59.77734375" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" width="31.77734375" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" width="80.109375" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" width="81.21875" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" width="134.33203125" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" width="48.33203125" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="66.7109375" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" width="69.7109375" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" width="31.77734375" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" width="80.109375" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" width="81.21875" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" width="134.33203125" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" width="48.33203125" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3364,24 +3886,36 @@
         <v>48</v>
       </c>
       <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3395,25 +3929,31 @@
       <c r="C2" t="s">
         <v>195</v>
       </c>
-      <c r="D2" t="s">
-        <v>136</v>
+      <c r="D2">
+        <v>3</v>
       </c>
       <c r="E2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F2" t="s">
+        <v>488</v>
+      </c>
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J2">
+      <c r="N2">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3424,7 +3964,10 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C3" t="s">
+        <v>770</v>
+      </c>
+      <c r="I3" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3435,11 +3978,14 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C4" t="s">
+        <v>768</v>
+      </c>
+      <c r="I4" t="s">
         <v>204</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -3448,7 +3994,10 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C5" t="s">
+        <v>769</v>
+      </c>
+      <c r="I5" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3459,7 +4008,10 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C6" t="s">
+        <v>766</v>
+      </c>
+      <c r="I6" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3470,7 +4022,10 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C7" t="s">
+        <v>767</v>
+      </c>
+      <c r="I7" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3483,22 +4038,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="D1" tabSelected="1">
-      <selection activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView workbookViewId="0" topLeftCell="A15" zoomScale="40" zoomScaleNormal="40" tabSelected="1">
+      <selection activeCell="O24" activeCellId="0" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" width="59.88671875" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" width="70.44140625" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" width="64.5703125" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" width="79.7109375" customWidth="1" bestFit="1"/>
     <col min="5" max="5" width="5.5546875" customWidth="1" bestFit="1"/>
     <col min="6" max="6" width="5.5546875" customWidth="1"/>
     <col min="7" max="7" width="5.5546875" customWidth="1"/>
     <col min="8" max="8" width="5.5546875" customWidth="1"/>
     <col min="9" max="9" width="25.109375" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" width="114" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" width="128.28515625" customWidth="1" bestFit="1"/>
     <col min="11" max="11" width="108.88671875" customWidth="1" bestFit="1"/>
     <col min="12" max="12" width="84.21875" customWidth="1" bestFit="1"/>
     <col min="15" max="15" width="82.33203125" customWidth="1" bestFit="1"/>
@@ -3558,6 +4113,12 @@
       <c r="B2" t="s">
         <v>660</v>
       </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>733</v>
+      </c>
       <c r="E2">
         <v>4</v>
       </c>
@@ -3599,6 +4160,12 @@
       <c r="B3" t="s">
         <v>661</v>
       </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>739</v>
+      </c>
       <c r="E3">
         <v>2</v>
       </c>
@@ -3634,11 +4201,32 @@
       <c r="B4" t="s">
         <v>662</v>
       </c>
+      <c r="C4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" t="s">
+        <v>740</v>
+      </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
         <v>400</v>
+      </c>
+      <c r="I4" t="s">
+        <v>691</v>
+      </c>
+      <c r="J4" t="s">
+        <v>692</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="5">
@@ -3648,6 +4236,33 @@
       <c r="B5" t="s">
         <v>663</v>
       </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
+        <v>741</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>400</v>
+      </c>
+      <c r="I5" t="s">
+        <v>691</v>
+      </c>
+      <c r="J5" t="s">
+        <v>694</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="55" t="s">
@@ -3656,6 +4271,33 @@
       <c r="B6" t="s">
         <v>664</v>
       </c>
+      <c r="C6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" t="s">
+        <v>742</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>400</v>
+      </c>
+      <c r="I6" t="s">
+        <v>691</v>
+      </c>
+      <c r="J6" t="s">
+        <v>696</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="55" t="s">
@@ -3664,6 +4306,33 @@
       <c r="B7" t="s">
         <v>665</v>
       </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>743</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>400</v>
+      </c>
+      <c r="I7" t="s">
+        <v>691</v>
+      </c>
+      <c r="J7" t="s">
+        <v>697</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="55" t="s">
@@ -3672,6 +4341,33 @@
       <c r="B8" t="s">
         <v>666</v>
       </c>
+      <c r="C8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" t="s">
+        <v>744</v>
+      </c>
+      <c r="F8" t="s">
+        <v>400</v>
+      </c>
+      <c r="G8" t="s">
+        <v>400</v>
+      </c>
+      <c r="I8" t="s">
+        <v>691</v>
+      </c>
+      <c r="J8" t="s">
+        <v>698</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="55" t="s">
@@ -3680,6 +4376,33 @@
       <c r="B9" t="s">
         <v>667</v>
       </c>
+      <c r="C9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" t="s">
+        <v>745</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>400</v>
+      </c>
+      <c r="I9" t="s">
+        <v>691</v>
+      </c>
+      <c r="J9" t="s">
+        <v>699</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="55" t="s">
@@ -3688,6 +4411,33 @@
       <c r="B10" t="s">
         <v>668</v>
       </c>
+      <c r="C10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" t="s">
+        <v>746</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>400</v>
+      </c>
+      <c r="I10" t="s">
+        <v>691</v>
+      </c>
+      <c r="J10" t="s">
+        <v>701</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="55" t="s">
@@ -3696,6 +4446,39 @@
       <c r="B11" t="s">
         <v>669</v>
       </c>
+      <c r="C11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" t="s">
+        <v>747</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>400</v>
+      </c>
+      <c r="G11" t="s">
+        <v>400</v>
+      </c>
+      <c r="H11" t="s">
+        <v>400</v>
+      </c>
+      <c r="I11" t="s">
+        <v>691</v>
+      </c>
+      <c r="J11" t="s">
+        <v>702</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="55" t="s">
@@ -3704,6 +4487,33 @@
       <c r="B12" t="s">
         <v>670</v>
       </c>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" t="s">
+        <v>748</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>400</v>
+      </c>
+      <c r="I12" t="s">
+        <v>691</v>
+      </c>
+      <c r="J12" t="s">
+        <v>703</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="55" t="s">
@@ -3712,6 +4522,33 @@
       <c r="B13" t="s">
         <v>671</v>
       </c>
+      <c r="C13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" t="s">
+        <v>749</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>400</v>
+      </c>
+      <c r="I13" t="s">
+        <v>691</v>
+      </c>
+      <c r="J13" t="s">
+        <v>704</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="55" t="s">
@@ -3720,6 +4557,36 @@
       <c r="B14" t="s">
         <v>672</v>
       </c>
+      <c r="C14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" t="s">
+        <v>750</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>400</v>
+      </c>
+      <c r="G14" t="s">
+        <v>400</v>
+      </c>
+      <c r="I14" t="s">
+        <v>691</v>
+      </c>
+      <c r="J14" t="s">
+        <v>705</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="55" t="s">
@@ -3728,6 +4595,30 @@
       <c r="B15" t="s">
         <v>673</v>
       </c>
+      <c r="C15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D15" t="s">
+        <v>751</v>
+      </c>
+      <c r="F15" t="s">
+        <v>400</v>
+      </c>
+      <c r="I15" t="s">
+        <v>691</v>
+      </c>
+      <c r="J15" t="s">
+        <v>706</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="55" t="s">
@@ -3736,6 +4627,39 @@
       <c r="B16" t="s">
         <v>674</v>
       </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>752</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>400</v>
+      </c>
+      <c r="G16" t="s">
+        <v>400</v>
+      </c>
+      <c r="H16" t="s">
+        <v>400</v>
+      </c>
+      <c r="I16" t="s">
+        <v>691</v>
+      </c>
+      <c r="J16" t="s">
+        <v>707</v>
+      </c>
+      <c r="M16">
+        <v>8</v>
+      </c>
+      <c r="N16">
+        <v>6</v>
+      </c>
+      <c r="O16" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="55" t="s">
@@ -3744,6 +4668,33 @@
       <c r="B17" t="s">
         <v>675</v>
       </c>
+      <c r="C17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" t="s">
+        <v>753</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>400</v>
+      </c>
+      <c r="I17" t="s">
+        <v>691</v>
+      </c>
+      <c r="J17" t="s">
+        <v>708</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>4</v>
+      </c>
+      <c r="O17" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="55" t="s">
@@ -3752,6 +4703,33 @@
       <c r="B18" t="s">
         <v>676</v>
       </c>
+      <c r="C18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" t="s">
+        <v>754</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>400</v>
+      </c>
+      <c r="I18" t="s">
+        <v>691</v>
+      </c>
+      <c r="J18" t="s">
+        <v>709</v>
+      </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="55" t="s">
@@ -3760,6 +4738,36 @@
       <c r="B19" t="s">
         <v>677</v>
       </c>
+      <c r="C19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" t="s">
+        <v>755</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>400</v>
+      </c>
+      <c r="G19" t="s">
+        <v>400</v>
+      </c>
+      <c r="I19" t="s">
+        <v>691</v>
+      </c>
+      <c r="J19" t="s">
+        <v>710</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>5</v>
+      </c>
+      <c r="O19" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="55" t="s">
@@ -3768,6 +4776,36 @@
       <c r="B20" t="s">
         <v>678</v>
       </c>
+      <c r="C20" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" t="s">
+        <v>756</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>400</v>
+      </c>
+      <c r="G20" t="s">
+        <v>400</v>
+      </c>
+      <c r="I20" t="s">
+        <v>691</v>
+      </c>
+      <c r="J20" t="s">
+        <v>711</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>6</v>
+      </c>
+      <c r="O20" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="55" t="s">
@@ -3776,6 +4814,33 @@
       <c r="B21" t="s">
         <v>679</v>
       </c>
+      <c r="C21" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" t="s">
+        <v>757</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>400</v>
+      </c>
+      <c r="I21" t="s">
+        <v>691</v>
+      </c>
+      <c r="J21" t="s">
+        <v>712</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="O21" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="55" t="s">
@@ -3784,6 +4849,36 @@
       <c r="B22" t="s">
         <v>680</v>
       </c>
+      <c r="C22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" t="s">
+        <v>758</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>400</v>
+      </c>
+      <c r="G22" t="s">
+        <v>400</v>
+      </c>
+      <c r="I22" t="s">
+        <v>691</v>
+      </c>
+      <c r="J22" t="s">
+        <v>713</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+      <c r="N22">
+        <v>5</v>
+      </c>
+      <c r="O22" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="55" t="s">
@@ -3791,6 +4886,874 @@
       </c>
       <c r="B23" t="s">
         <v>681</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>759</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>400</v>
+      </c>
+      <c r="G23" t="s">
+        <v>400</v>
+      </c>
+      <c r="H23" t="s">
+        <v>400</v>
+      </c>
+      <c r="I23" t="s">
+        <v>691</v>
+      </c>
+      <c r="J23" t="s">
+        <v>714</v>
+      </c>
+      <c r="M23">
+        <v>7</v>
+      </c>
+      <c r="N23">
+        <v>7</v>
+      </c>
+      <c r="O23" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B24" t="s">
+        <v>794</v>
+      </c>
+      <c r="C24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D24" t="s">
+        <v>796</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>487</v>
+      </c>
+      <c r="I24" t="s">
+        <v>819</v>
+      </c>
+      <c r="J24" t="s">
+        <v>843</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B25" t="s">
+        <v>793</v>
+      </c>
+      <c r="C25" t="s">
+        <v>211</v>
+      </c>
+      <c r="D25" t="s">
+        <v>797</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>487</v>
+      </c>
+      <c r="I25" t="s">
+        <v>819</v>
+      </c>
+      <c r="J25" t="s">
+        <v>842</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>4</v>
+      </c>
+      <c r="O25" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B26" t="s">
+        <v>792</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>798</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>487</v>
+      </c>
+      <c r="G26" t="s">
+        <v>487</v>
+      </c>
+      <c r="H26" t="s">
+        <v>487</v>
+      </c>
+      <c r="I26" t="s">
+        <v>819</v>
+      </c>
+      <c r="J26" t="s">
+        <v>841</v>
+      </c>
+      <c r="M26">
+        <v>6</v>
+      </c>
+      <c r="N26">
+        <v>6</v>
+      </c>
+      <c r="O26" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B27" t="s">
+        <v>791</v>
+      </c>
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" t="s">
+        <v>799</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>487</v>
+      </c>
+      <c r="I27" t="s">
+        <v>819</v>
+      </c>
+      <c r="J27" t="s">
+        <v>840</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" t="s">
+        <v>790</v>
+      </c>
+      <c r="C28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" t="s">
+        <v>800</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>487</v>
+      </c>
+      <c r="I28" t="s">
+        <v>819</v>
+      </c>
+      <c r="J28" t="s">
+        <v>839</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B29" t="s">
+        <v>789</v>
+      </c>
+      <c r="C29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D29" t="s">
+        <v>801</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>487</v>
+      </c>
+      <c r="G29" t="s">
+        <v>487</v>
+      </c>
+      <c r="I29" t="s">
+        <v>819</v>
+      </c>
+      <c r="J29" t="s">
+        <v>838</v>
+      </c>
+      <c r="M29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B30" t="s">
+        <v>788</v>
+      </c>
+      <c r="C30" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" t="s">
+        <v>802</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>487</v>
+      </c>
+      <c r="I30" t="s">
+        <v>819</v>
+      </c>
+      <c r="J30" t="s">
+        <v>837</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="N30">
+        <v>5</v>
+      </c>
+      <c r="O30" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B31" t="s">
+        <v>787</v>
+      </c>
+      <c r="C31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" t="s">
+        <v>803</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>487</v>
+      </c>
+      <c r="I31" t="s">
+        <v>819</v>
+      </c>
+      <c r="J31" t="s">
+        <v>836</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B32" t="s">
+        <v>786</v>
+      </c>
+      <c r="C32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32" t="s">
+        <v>804</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>487</v>
+      </c>
+      <c r="G32" t="s">
+        <v>487</v>
+      </c>
+      <c r="I32" t="s">
+        <v>819</v>
+      </c>
+      <c r="J32" t="s">
+        <v>835</v>
+      </c>
+      <c r="M32">
+        <v>5</v>
+      </c>
+      <c r="N32">
+        <v>4</v>
+      </c>
+      <c r="O32" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B33" t="s">
+        <v>785</v>
+      </c>
+      <c r="C33" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" t="s">
+        <v>805</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>487</v>
+      </c>
+      <c r="I33" t="s">
+        <v>819</v>
+      </c>
+      <c r="J33" t="s">
+        <v>834</v>
+      </c>
+      <c r="M33">
+        <v>3</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+      <c r="O33" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B34" t="s">
+        <v>784</v>
+      </c>
+      <c r="C34" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" t="s">
+        <v>806</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>487</v>
+      </c>
+      <c r="I34" t="s">
+        <v>819</v>
+      </c>
+      <c r="J34" t="s">
+        <v>833</v>
+      </c>
+      <c r="M34">
+        <v>3</v>
+      </c>
+      <c r="N34">
+        <v>6</v>
+      </c>
+      <c r="O34" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B35" t="s">
+        <v>783</v>
+      </c>
+      <c r="C35" t="s">
+        <v>215</v>
+      </c>
+      <c r="D35" t="s">
+        <v>807</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>487</v>
+      </c>
+      <c r="G35" t="s">
+        <v>487</v>
+      </c>
+      <c r="I35" t="s">
+        <v>819</v>
+      </c>
+      <c r="J35" t="s">
+        <v>832</v>
+      </c>
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="O35" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B36" t="s">
+        <v>782</v>
+      </c>
+      <c r="C36" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" t="s">
+        <v>808</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>487</v>
+      </c>
+      <c r="I36" t="s">
+        <v>819</v>
+      </c>
+      <c r="J36" t="s">
+        <v>831</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36">
+        <v>2</v>
+      </c>
+      <c r="O36" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B37" t="s">
+        <v>781</v>
+      </c>
+      <c r="C37" t="s">
+        <v>215</v>
+      </c>
+      <c r="D37" t="s">
+        <v>809</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>487</v>
+      </c>
+      <c r="I37" t="s">
+        <v>819</v>
+      </c>
+      <c r="J37" t="s">
+        <v>830</v>
+      </c>
+      <c r="M37">
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <v>5</v>
+      </c>
+      <c r="O37" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" t="s">
+        <v>780</v>
+      </c>
+      <c r="C38" t="s">
+        <v>209</v>
+      </c>
+      <c r="D38" t="s">
+        <v>810</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>487</v>
+      </c>
+      <c r="I38" t="s">
+        <v>819</v>
+      </c>
+      <c r="J38" t="s">
+        <v>829</v>
+      </c>
+      <c r="M38">
+        <v>2</v>
+      </c>
+      <c r="N38">
+        <v>3</v>
+      </c>
+      <c r="O38" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B39" t="s">
+        <v>779</v>
+      </c>
+      <c r="C39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D39" t="s">
+        <v>811</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>487</v>
+      </c>
+      <c r="I39" t="s">
+        <v>819</v>
+      </c>
+      <c r="J39" t="s">
+        <v>828</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+      <c r="O39" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B40" t="s">
+        <v>778</v>
+      </c>
+      <c r="C40" t="s">
+        <v>211</v>
+      </c>
+      <c r="D40" t="s">
+        <v>812</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>487</v>
+      </c>
+      <c r="I40" t="s">
+        <v>819</v>
+      </c>
+      <c r="J40" t="s">
+        <v>827</v>
+      </c>
+      <c r="M40">
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <v>2</v>
+      </c>
+      <c r="O40" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" t="s">
+        <v>777</v>
+      </c>
+      <c r="C41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D41" t="s">
+        <v>813</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>487</v>
+      </c>
+      <c r="G41" t="s">
+        <v>487</v>
+      </c>
+      <c r="I41" t="s">
+        <v>819</v>
+      </c>
+      <c r="J41" t="s">
+        <v>826</v>
+      </c>
+      <c r="M41">
+        <v>5</v>
+      </c>
+      <c r="N41">
+        <v>3</v>
+      </c>
+      <c r="O41" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B42" t="s">
+        <v>776</v>
+      </c>
+      <c r="C42" t="s">
+        <v>209</v>
+      </c>
+      <c r="D42" t="s">
+        <v>814</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>487</v>
+      </c>
+      <c r="I42" t="s">
+        <v>819</v>
+      </c>
+      <c r="J42" t="s">
+        <v>825</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B43" t="s">
+        <v>775</v>
+      </c>
+      <c r="C43" t="s">
+        <v>215</v>
+      </c>
+      <c r="D43" t="s">
+        <v>815</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>487</v>
+      </c>
+      <c r="G43" t="s">
+        <v>487</v>
+      </c>
+      <c r="I43" t="s">
+        <v>819</v>
+      </c>
+      <c r="J43" t="s">
+        <v>824</v>
+      </c>
+      <c r="M43">
+        <v>4</v>
+      </c>
+      <c r="N43">
+        <v>6</v>
+      </c>
+      <c r="O43" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" t="s">
+        <v>774</v>
+      </c>
+      <c r="C44" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" t="s">
+        <v>816</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>487</v>
+      </c>
+      <c r="G44" t="s">
+        <v>487</v>
+      </c>
+      <c r="I44" t="s">
+        <v>819</v>
+      </c>
+      <c r="J44" t="s">
+        <v>823</v>
+      </c>
+      <c r="M44">
+        <v>3</v>
+      </c>
+      <c r="N44">
+        <v>4</v>
+      </c>
+      <c r="O44" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B45" t="s">
+        <v>773</v>
+      </c>
+      <c r="C45" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45" t="s">
+        <v>817</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>487</v>
+      </c>
+      <c r="I45" t="s">
+        <v>819</v>
+      </c>
+      <c r="J45" t="s">
+        <v>822</v>
+      </c>
+      <c r="M45">
+        <v>4</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+      <c r="O45" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B46" t="s">
+        <v>772</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>818</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>487</v>
+      </c>
+      <c r="G46" t="s">
+        <v>487</v>
+      </c>
+      <c r="H46" t="s">
+        <v>487</v>
+      </c>
+      <c r="I46" t="s">
+        <v>819</v>
+      </c>
+      <c r="J46" t="s">
+        <v>821</v>
+      </c>
+      <c r="M46">
+        <v>5</v>
+      </c>
+      <c r="N46">
+        <v>5</v>
+      </c>
+      <c r="O46" t="s">
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -3801,8 +5764,8 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1" zoomScale="110" zoomScaleNormal="110">
-      <selection activeCell="N91" activeCellId="0" sqref="N91"/>
+    <sheetView workbookViewId="0" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80">
+      <selection activeCell="A17" activeCellId="0" sqref="A17:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" customHeight="false"/>
@@ -5736,7 +7699,7 @@
         <v>395</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>539</v>
+        <v>760</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -5797,7 +7760,7 @@
         <v>395</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>541</v>
+        <v>761</v>
       </c>
       <c r="E67">
         <v>1</v>

</xml_diff>